<commit_message>
Include Formula in output
</commit_message>
<xml_diff>
--- a/testfile.xlsx
+++ b/testfile.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
-  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17927"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="20460" tabRatio="478"/>
   </bookViews>
@@ -11,7 +11,7 @@
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -23,10 +23,10 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Autor</author>
+    <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0">
+    <comment ref="A2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -52,7 +52,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A4" authorId="0">
+    <comment ref="A4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -190,9 +190,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -264,6 +264,14 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -589,13 +597,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -603,12 +614,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
+      </c>
+      <c r="C2" t="str">
+        <f>LOWER(B2)</f>
+        <v>quuk</v>
       </c>
     </row>
   </sheetData>
@@ -624,14 +639,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A2:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:1"/>
-    <row r="4" spans="1:1"/>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -646,11 +662,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>